<commit_message>
added hypothesis's and the conclusions of the tests on whether or not I can reject the null hypothesis
</commit_message>
<xml_diff>
--- a/t-test accuracy results/rocket_two_tailed_t-tests.xlsx
+++ b/t-test accuracy results/rocket_two_tailed_t-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redma\Documents\GitHub\ExerciseClassification\t-test accuracy results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716D565F-7984-4EC7-A6D6-CF16E9FCA493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B0B064-D84B-46BC-B2E8-34709CFE5C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="47">
   <si>
     <t>Rocket</t>
   </si>
@@ -122,6 +122,66 @@
   </si>
   <si>
     <t>Time Series Forest</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and AdaBoost on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and AdaBoost on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and Boss Ensemble on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and Boss Ensemble on gym movements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based off the evidence of this test we cannot reject the null hypothesis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based off the evidence of this test we can reject the null hypothesis </t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and Decision Tree on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and Decision Tree on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and kNN-ED on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and kNN-ED on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and kNN-DTW on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and kNN-DTW on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and MLP on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and MLP on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and Naïve Bayes on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and Naïve Bayes on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and Random Forest on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and Random Forest on gym movements</t>
+  </si>
+  <si>
+    <t>H0: there is no difference in mean accuracry between Rocket and Time Series Forest on gym movements</t>
+  </si>
+  <si>
+    <t>H1: there is a difference in mean accuracry between Rocket and Time Series Forest on gym movements</t>
   </si>
 </sst>
 </file>
@@ -225,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -243,6 +303,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181FC21C-74BD-47D5-A002-640CBAB53DA8}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F16"/>
+      <selection activeCell="H20" sqref="A17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,7 +906,46 @@
       </c>
       <c r="J15" s="9"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -851,10 +953,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92284911-FCE9-44E5-9B43-052B0FBAF35E}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="A1:F12"/>
+      <selection activeCell="H20" sqref="A17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,17 +1251,56 @@
       </c>
       <c r="J15" s="9"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C0E2C9-E4E1-4688-B2FF-976D27B553B5}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H20" sqref="A17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1454,17 +1595,56 @@
       </c>
       <c r="J15" s="9"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE44B29-F965-4C4A-9712-4206BA7CEE4F}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H20" sqref="A17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1759,7 +1939,46 @@
       </c>
       <c r="J15" s="9"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1769,10 +1988,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="A1:F13"/>
+      <selection activeCell="A17" sqref="A17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2072,27 +2291,70 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.3">
-      <c r="H17" s="8"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.3">
-      <c r="H18" s="12"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52310191-8F49-410A-9D3A-8D0D1377F310}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="A1:F11"/>
+      <selection activeCell="H20" sqref="A17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2397,17 +2659,56 @@
       </c>
       <c r="J15" s="9"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EF8C36-7090-464D-AAB3-3C1E05473A40}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="A1:F12"/>
+      <selection activeCell="H20" sqref="A17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2703,17 +3004,56 @@
       </c>
       <c r="J15" s="9"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3A3F0C-C3E2-4E4D-B618-BC26E5093D91}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="H20" sqref="A17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3008,17 +3348,56 @@
       </c>
       <c r="J15" s="9"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F920CD64-38D7-4C34-AE1D-7F46FDF00FF8}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3314,7 +3693,46 @@
       </c>
       <c r="J15" s="9"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:F20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>